<commit_message>
Replaced is_ideal_scale() for a simpler function that prints both adjacent units for individual comparison
</commit_message>
<xml_diff>
--- a/Information_Reference/Convert Chart.xlsx
+++ b/Information_Reference/Convert Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Starship_Bloopers\Information_Reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2155351D-D16C-4FA1-BDBB-7CE088015056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C51593-1DD7-44C0-A7DF-8DD51B1221A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{EED035EF-18E1-45E5-84F9-AA6FD0A16076}"/>
+    <workbookView xWindow="-16305" yWindow="-2550" windowWidth="16410" windowHeight="14145" xr2:uid="{EED035EF-18E1-45E5-84F9-AA6FD0A16076}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -106,9 +106,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -448,7 +449,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,27 +497,27 @@
       <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <f>1/B3</f>
         <v>1E-3</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <f>1/B4</f>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <f>1/B5</f>
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="3">
         <f>1/B6</f>
         <v>6.684581344670383E-12</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="3">
         <f>1/B7</f>
         <v>1.0569995374322052E-16</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="3">
         <f>1/B8</f>
         <v>3.2407790671709406E-17</v>
       </c>
@@ -531,23 +532,23 @@
       <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <f>1/C4</f>
         <v>1E-3</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <f>1/C5</f>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="3">
         <f>1/C6</f>
         <v>6.6845813446703832E-9</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="3">
         <f>1/C7</f>
         <v>1.0569995374322053E-13</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="3">
         <f>1/C8</f>
         <v>3.2407790671709404E-14</v>
       </c>
@@ -566,19 +567,19 @@
       <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <f>1/D5</f>
         <v>1E-3</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="3">
         <f>1/D6</f>
         <v>6.684581344670383E-6</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="3">
         <f>1/D7</f>
         <v>1.0569995374322053E-10</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="3">
         <f>1/D8</f>
         <v>3.2407790671709404E-11</v>
       </c>
@@ -601,15 +602,15 @@
       <c r="E5" s="2">
         <v>1</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="3">
         <f>1/E6</f>
         <v>6.6845813446703827E-3</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="3">
         <f>1/E7</f>
         <v>1.0569995374322052E-7</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="3">
         <f>1/E8</f>
         <v>3.2407790671709403E-8</v>
       </c>
@@ -636,11 +637,11 @@
       <c r="F6" s="2">
         <v>1</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="3">
         <f>1/F7</f>
         <v>1.5812501680078302E-5</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="3">
         <f>1/F8</f>
         <v>4.8481406689063836E-6</v>
       </c>
@@ -671,7 +672,7 @@
       <c r="G7" s="2">
         <v>1</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="3">
         <f>1/G8</f>
         <v>0.30660174885637548</v>
       </c>

</xml_diff>